<commit_message>
Update Database.java / ServerConnectTask.java / CareerSuccessFragment.java / graduation_info_list.xlsx
added 공학인증
</commit_message>
<xml_diff>
--- a/app/src/main/res/raw/graduation_info_list.xlsx
+++ b/app/src/main/res/raw/graduation_info_list.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\knuGra\app\src\main\res\raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gihub\knuGra\app\src\main\res\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{030CD1F0-1C56-4BCD-8A5D-BF17D6920CC1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4353F791-71F0-4096-8AB9-37443355F326}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="16395" windowHeight="27481" xr2:uid="{D23521AE-361F-4FFE-95A8-7F1CDDEB2FB7}"/>
+    <workbookView xWindow="9780" yWindow="1245" windowWidth="21600" windowHeight="11385" xr2:uid="{D23521AE-361F-4FFE-95A8-7F1CDDEB2FB7}"/>
   </bookViews>
   <sheets>
     <sheet name="심화컴퓨터전공(ABEEK)" sheetId="1" r:id="rId1"/>
@@ -21,8 +21,8 @@
     <sheet name="건설IT전공" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">글로벌소프트웨어전공!$A$1:$B$21</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'심화컴퓨터전공(ABEEK)'!$A$1:$B$22</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">글로벌소프트웨어전공!$A$1:$B$20</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'심화컴퓨터전공(ABEEK)'!$A$1:$B$21</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="22">
   <si>
     <t>상담</t>
   </si>
@@ -68,13 +68,7 @@
     <t>기본소양</t>
   </si>
   <si>
-    <t>이수합계</t>
-  </si>
-  <si>
     <t>전공기반</t>
-  </si>
-  <si>
-    <t>평점평균</t>
   </si>
   <si>
     <t>현장실습</t>
@@ -95,6 +89,34 @@
   </si>
   <si>
     <t>전공</t>
+  </si>
+  <si>
+    <t>이수학점</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pass</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>공학상담</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기본소양</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>공학인증</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>전공기반</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>공학전공</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -458,101 +480,93 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F5D8F4F-A3EB-4C52-9B1A-6ED05ED44471}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.899999999999999" x14ac:dyDescent="0.6"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="19.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.6">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="B2">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.6">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="B3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6">
         <v>112</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A6" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>1</v>
       </c>
-      <c r="B6">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>9</v>
       </c>
       <c r="B8">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B9">
-        <v>1.7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B22" xr:uid="{55D4EBA4-2028-42B0-B2AD-A98A4F2019FA}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B22">
-      <sortCondition ref="A1:A22"/>
+  <autoFilter ref="A1:B21" xr:uid="{55D4EBA4-2028-42B0-B2AD-A98A4F2019FA}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B21">
+      <sortCondition ref="A1:A21"/>
     </sortState>
   </autoFilter>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -563,34 +577,34 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FD99409-18A7-49CB-BF27-87F2247D7B4A}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C68" sqref="C68"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.899999999999999" x14ac:dyDescent="0.6"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="20.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>12</v>
-      </c>
-      <c r="B1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A2" t="s">
-        <v>14</v>
       </c>
       <c r="B2">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -598,15 +612,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -614,23 +628,23 @@
         <v>700</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B6">
         <v>130</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B7">
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -638,49 +652,117 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B9">
-        <v>1.7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10">
         <v>3</v>
       </c>
-      <c r="B10">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11">
-        <v>3</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B21" xr:uid="{955A4EBC-36E8-47D9-A668-16F00873580E}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B21">
-      <sortCondition ref="A1:A21"/>
+  <autoFilter ref="A1:B20" xr:uid="{955A4EBC-36E8-47D9-A668-16F00873580E}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B20">
+      <sortCondition ref="A1:A20"/>
     </sortState>
   </autoFilter>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6531C50E-98D0-4AD5-B146-E35B9A6CCC2F}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.899999999999999" x14ac:dyDescent="0.6"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -694,7 +776,7 @@
       <selection activeCell="H60" sqref="H60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.899999999999999" x14ac:dyDescent="0.6"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -707,7 +789,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.899999999999999" x14ac:dyDescent="0.6"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -722,7 +804,7 @@
       <selection activeCell="F65" sqref="F65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.899999999999999" x14ac:dyDescent="0.6"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update DAPATH / Database / Graduation_Info_List / graduation_info_list.xlsx / required_subject_list.xlsx
added Global SW major data
</commit_message>
<xml_diff>
--- a/app/src/main/res/raw/graduation_info_list.xlsx
+++ b/app/src/main/res/raw/graduation_info_list.xlsx
@@ -5,23 +5,25 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gihub\knuGra\app\src\main\res\raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\knuGra\app\src\main\res\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4353F791-71F0-4096-8AB9-37443355F326}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C689C6A-CD39-4F2A-BA0F-5EAA177DB7AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9780" yWindow="1245" windowWidth="21600" windowHeight="11385" xr2:uid="{D23521AE-361F-4FFE-95A8-7F1CDDEB2FB7}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12181" tabRatio="709" firstSheet="1" activeTab="1" xr2:uid="{D23521AE-361F-4FFE-95A8-7F1CDDEB2FB7}"/>
   </bookViews>
   <sheets>
     <sheet name="심화컴퓨터전공(ABEEK)" sheetId="1" r:id="rId1"/>
-    <sheet name="글로벌소프트웨어전공" sheetId="2" r:id="rId2"/>
-    <sheet name="핀테크전공" sheetId="3" r:id="rId3"/>
-    <sheet name="빅데이터전공" sheetId="4" r:id="rId4"/>
-    <sheet name="미디어아트" sheetId="5" r:id="rId5"/>
-    <sheet name="건설IT전공" sheetId="6" r:id="rId6"/>
+    <sheet name="글로벌소프트웨어전공(다중전공트랙)" sheetId="2" r:id="rId2"/>
+    <sheet name="글로벌소프트웨어전공(해외복수학위트랙)" sheetId="7" r:id="rId3"/>
+    <sheet name="글로벌소프트웨어전공(학석사연계트랙)" sheetId="8" r:id="rId4"/>
+    <sheet name="핀테크전공" sheetId="3" r:id="rId5"/>
+    <sheet name="빅데이터전공" sheetId="4" r:id="rId6"/>
+    <sheet name="미디어아트" sheetId="5" r:id="rId7"/>
+    <sheet name="건설IT전공" sheetId="6" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">글로벌소프트웨어전공!$A$1:$B$20</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'글로벌소프트웨어전공(다중전공트랙)'!$A$1:$B$20</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'심화컴퓨터전공(ABEEK)'!$A$1:$B$21</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -42,80 +44,106 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="28">
+  <si>
+    <t>영어성적</t>
+  </si>
+  <si>
+    <t>창업역량</t>
+  </si>
+  <si>
+    <t>공학상담</t>
+  </si>
+  <si>
+    <t>공학인증</t>
+  </si>
+  <si>
+    <t>공학전공</t>
+  </si>
+  <si>
+    <t>기본소양</t>
+  </si>
+  <si>
+    <t>전공기반</t>
+  </si>
+  <si>
+    <t>현장실습</t>
+  </si>
+  <si>
+    <t>구분</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>값</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>교양</t>
+  </si>
+  <si>
+    <t>스타트업</t>
+  </si>
+  <si>
+    <t>전공</t>
+  </si>
+  <si>
+    <t>이수학점</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pass</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>공학상담</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기본소양</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>공학인증</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>전공기반</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>공학전공</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>해외역량</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
   <si>
     <t>상담</t>
-  </si>
-  <si>
-    <t>영어성적</t>
-  </si>
-  <si>
-    <t>창업역량</t>
-  </si>
-  <si>
-    <t>해외역량</t>
-  </si>
-  <si>
-    <t>공학상담</t>
-  </si>
-  <si>
-    <t>공학인증</t>
-  </si>
-  <si>
-    <t>공학전공</t>
-  </si>
-  <si>
-    <t>기본소양</t>
-  </si>
-  <si>
-    <t>전공기반</t>
-  </si>
-  <si>
-    <t>현장실습</t>
-  </si>
-  <si>
-    <t>구분</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>값</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>교양</t>
-  </si>
-  <si>
-    <t>스타트업</t>
-  </si>
-  <si>
-    <t>전공</t>
-  </si>
-  <si>
-    <t>이수학점</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>pass</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>공학상담</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>기본소양</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>공학인증</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>전공기반</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>공학전공</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>융합전공</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>연계전공</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>복수전공</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>부전공</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>복수학위취득</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>창업</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -482,82 +510,82 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F5D8F4F-A3EB-4C52-9B1A-6ED05ED44471}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.899999999999999" x14ac:dyDescent="0.6"/>
   <cols>
     <col min="1" max="2" width="19.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B2">
         <v>150</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B3">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B4">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B5">
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B6">
         <v>112</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A7" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B8">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -577,95 +605,127 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FD99409-18A7-49CB-BF27-87F2247D7B4A}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.899999999999999" x14ac:dyDescent="0.6"/>
   <cols>
     <col min="1" max="2" width="20.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2">
+      <c r="B5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A13" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7">
+      <c r="B13">
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10">
-        <v>3</v>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -681,6 +741,166 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E116890-BBC2-47A2-BEFB-5123B6B8749B}">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.899999999999999" x14ac:dyDescent="0.6"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFA7DF61-694A-44AF-B5B5-53E98ED994CD}">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.899999999999999" x14ac:dyDescent="0.6"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6531C50E-98D0-4AD5-B146-E35B9A6CCC2F}">
   <dimension ref="A1:B9"/>
   <sheetViews>
@@ -688,75 +908,75 @@
       <selection sqref="A1:B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.899999999999999" x14ac:dyDescent="0.6"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B2">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B3">
         <v>112</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B4">
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B5">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B7">
         <v>150</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>3</v>
@@ -768,7 +988,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E15722BC-B5DD-4187-9DCA-2B6A17B4C937}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -776,27 +996,27 @@
       <selection activeCell="H60" sqref="H60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.899999999999999" x14ac:dyDescent="0.6"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78E7CAEE-5FE8-430A-8741-954F9EA41F2E}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.899999999999999" x14ac:dyDescent="0.6"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A617C373-4E2F-4FD3-A55D-888795D8A974}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -804,7 +1024,7 @@
       <selection activeCell="F65" sqref="F65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.899999999999999" x14ac:dyDescent="0.6"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>